<commit_message>
zero-excel finished, import data
</commit_message>
<xml_diff>
--- a/vertx-zeus/up-ares/src/main/resources/plugin/excel/data/DATA-USER.xlsx
+++ b/vertx-zeus/up-ares/src/main/resources/plugin/excel/data/DATA-USER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/vertx-zero/vertx-zeus/up-ares/src/main/resources/plugin/excel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9C3B05-43FF-D141-91D0-D93F42D8441D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FDB79D-8702-AA47-9960-C8FB709B372F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>active</t>
   </si>
@@ -59,15 +59,9 @@
     <t>8c148b72-7348-4d4e-b604-3b7d6053ac1e</t>
   </si>
   <si>
-    <t>I_API</t>
-  </si>
-  <si>
     <t>9744ae98-eac1-4825-b558-3e53c78940da</t>
   </si>
   <si>
-    <t>cn.vertxup.domain.tables.daos.SUserDao</t>
-  </si>
-  <si>
     <t>用户账号</t>
   </si>
   <si>
@@ -129,6 +123,18 @@
   </si>
   <si>
     <t>15922611448</t>
+  </si>
+  <si>
+    <t>S_USER</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>统一标识符</t>
+  </si>
+  <si>
+    <t>kbm9LQBAsm8BPJQ7AIG9MVDgaF7azrWd</t>
   </si>
 </sst>
 </file>
@@ -198,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -221,49 +227,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -278,7 +247,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,13 +289,7 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -645,157 +607,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE8EFB5-630A-0B48-8E56-AEAA85248043}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.83203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="41.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="39.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="16" customWidth="1"/>
     <col min="6" max="6" width="26.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="12" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="7"/>
+    <col min="7" max="7" width="11.83203125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="12" style="6" customWidth="1"/>
+    <col min="9" max="9" width="46.5" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="2"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="17"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="16"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="13"/>
+      <c r="G1" s="12"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="15" t="s">
+      <c r="B6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="8" t="s">
+      <c r="G6" s="9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>3</v>
+      <c r="I6" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="C2:I2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" xr:uid="{493DFD13-924D-C948-A8A8-E24975239E6F}"/>

</xml_diff>